<commit_message>
Modify Task: nvidia-stock-analysis: change the time duration of needed data
</commit_message>
<xml_diff>
--- a/tasks/finalpool/nvidia-stock-analysis/initial_workspace/results_template.xlsx
+++ b/tasks/finalpool/nvidia-stock-analysis/initial_workspace/results_template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\CJP\Desktop\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/quentin/Desktop/RESEARCH/MCP/finalpool/mcpbench_dev/tasks/finalpool/nvidia-stock-analysis/initial_workspace/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7A8451-A0F6-4E98-9359-1521CEEE91C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDD6E82C-B258-7B4E-A36C-C5C4457E4930}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="780" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Basic Trend" sheetId="1" r:id="rId1"/>
@@ -22,81 +22,73 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Quarter</t>
   </si>
   <si>
-    <t>2023Q1</t>
-  </si>
-  <si>
-    <t>2023Q2</t>
-  </si>
-  <si>
-    <t>2023Q3</t>
-  </si>
-  <si>
-    <t>2023Q4</t>
-  </si>
-  <si>
-    <t>2024Q1</t>
-  </si>
-  <si>
-    <t>2024Q2</t>
+    <t>Shareholder Name</t>
+  </si>
+  <si>
+    <t>Holding Value (Billion USD)</t>
+  </si>
+  <si>
+    <t>Holding Ratio (%)</t>
+  </si>
+  <si>
+    <t>NVDA End-of-Quarter Stock Price (USD)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Outstanding Shares (Million Shares)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Shares Held (Million Shares)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Percentage Change (%)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Market Cap (Billion USD)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Indicator</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Insiders Held Percentage (%)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Institutions Held Percentage (%)</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>#Institutions</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>2024Q3</t>
+    <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
     <t>2024Q4</t>
-  </si>
-  <si>
-    <t>Shareholder Name</t>
-  </si>
-  <si>
-    <t>Holding Value (Billion USD)</t>
-  </si>
-  <si>
-    <t>Holding Ratio (%)</t>
-  </si>
-  <si>
-    <t>NVDA End-of-Quarter Stock Price (USD)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Outstanding Shares (Million Shares)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Shares Held (Million Shares)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Percentage Change (%)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Market Cap (Billion USD)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Indicator</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Insiders Held Percentage (%)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>Institutions Held Percentage (%)</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
-    <t>#Institutions</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025Q1</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2025Q2</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -104,7 +96,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -116,6 +108,7 @@
       <b/>
       <sz val="11"/>
       <name val="宋体"/>
+      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -478,72 +471,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
-    <col min="2" max="2" width="51.90625" customWidth="1"/>
-    <col min="3" max="3" width="60.08984375" customWidth="1"/>
-    <col min="4" max="4" width="51.81640625" customWidth="1"/>
+    <col min="1" max="1" width="14.1640625" customWidth="1"/>
+    <col min="2" max="2" width="51.83203125" customWidth="1"/>
+    <col min="3" max="3" width="60.1640625" customWidth="1"/>
+    <col min="4" max="4" width="51.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>8</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -561,33 +534,33 @@
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="69.7265625" customWidth="1"/>
-    <col min="2" max="2" width="51.7265625" customWidth="1"/>
+    <col min="1" max="1" width="69.6640625" customWidth="1"/>
+    <col min="2" max="2" width="51.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2">
       <c r="A1" s="2" t="s">
-        <v>18</v>
+        <v>10</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
       <c r="A3" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -604,30 +577,30 @@
       <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="22.08984375" customWidth="1"/>
-    <col min="2" max="2" width="43.26953125" customWidth="1"/>
-    <col min="3" max="3" width="32.26953125" customWidth="1"/>
-    <col min="4" max="4" width="26.6328125" customWidth="1"/>
-    <col min="5" max="5" width="53.1796875" customWidth="1"/>
+    <col min="1" max="1" width="22.1640625" customWidth="1"/>
+    <col min="2" max="2" width="43.33203125" customWidth="1"/>
+    <col min="3" max="3" width="32.33203125" customWidth="1"/>
+    <col min="4" max="4" width="26.6640625" customWidth="1"/>
+    <col min="5" max="5" width="53.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>11</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>